<commit_message>
Changed template for upload excel.
</commit_message>
<xml_diff>
--- a/web/code/plugins/http/assets/upload_file/Mol_upload_items.xlsx
+++ b/web/code/plugins/http/assets/upload_file/Mol_upload_items.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korakodc\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitLab\mol2016\web\code\plugins\http\public\upload_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,15 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>item_reference</t>
+  </si>
+  <si>
+    <t>order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,10 +347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -355,19 +358,52 @@
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1000000872</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1000012164</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1000000873</v>
+        <v>1000007500</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1000000676</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1000000633</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1000014725</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>